<commit_message>
Team data for 2020-21 season
</commit_message>
<xml_diff>
--- a/Team-Data/2020-21/1-1-2020-21.xlsx
+++ b/Team-Data/2020-21/1-1-2020-21.xlsx
@@ -1766,7 +1766,7 @@
         <v>11</v>
       </c>
       <c r="AS7" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AT7" t="n">
         <v>11</v>
@@ -2234,16 +2234,16 @@
         <v>12.4</v>
       </c>
       <c r="S10" t="n">
-        <v>35.8</v>
+        <v>36</v>
       </c>
       <c r="T10" t="n">
-        <v>48.2</v>
+        <v>48.4</v>
       </c>
       <c r="U10" t="n">
         <v>23.2</v>
       </c>
       <c r="V10" t="n">
-        <v>16.2</v>
+        <v>16.4</v>
       </c>
       <c r="W10" t="n">
         <v>7.6</v>
@@ -2315,13 +2315,13 @@
         <v>14</v>
       </c>
       <c r="AT10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AU10" t="n">
         <v>19</v>
       </c>
       <c r="AV10" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AW10" t="n">
         <v>19</v>
@@ -3225,13 +3225,13 @@
         <v>2</v>
       </c>
       <c r="AT15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AU15" t="n">
         <v>7</v>
       </c>
       <c r="AV15" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AW15" t="n">
         <v>26</v>
@@ -4135,7 +4135,7 @@
         <v>6</v>
       </c>
       <c r="AT20" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AU20" t="n">
         <v>29</v>
@@ -4678,7 +4678,7 @@
         <v>8</v>
       </c>
       <c r="AS23" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AT23" t="n">
         <v>10</v>
@@ -4863,7 +4863,7 @@
         <v>1</v>
       </c>
       <c r="AT24" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AU24" t="n">
         <v>24</v>
@@ -6143,7 +6143,7 @@
         <v>2</v>
       </c>
       <c r="AV31" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AW31" t="n">
         <v>23</v>

</xml_diff>

<commit_message>
More data for 2021-22 season
</commit_message>
<xml_diff>
--- a/Team-Data/2020-21/1-1-2020-21.xlsx
+++ b/Team-Data/2020-21/1-1-2020-21.xlsx
@@ -3049,16 +3049,16 @@
         <v>108</v>
       </c>
       <c r="BN3" t="n">
-        <v>108.9</v>
+        <v>108.7</v>
       </c>
       <c r="BO3" t="n">
-        <v>107.4</v>
+        <v>107.2</v>
       </c>
       <c r="BP3" t="n">
-        <v>109.7</v>
+        <v>109.5</v>
       </c>
       <c r="BQ3" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="BR3" t="n">
         <v>-0.8</v>
@@ -3073,13 +3073,13 @@
         <v>16.5</v>
       </c>
       <c r="BV3" t="n">
-        <v>0.279</v>
+        <v>0.276</v>
       </c>
       <c r="BW3" t="n">
         <v>0.707</v>
       </c>
       <c r="BX3" t="n">
-        <v>0.489</v>
+        <v>0.487</v>
       </c>
       <c r="BY3" t="n">
         <v>0.15</v>
@@ -3091,16 +3091,16 @@
         <v>0.5639999999999999</v>
       </c>
       <c r="CB3" t="n">
-        <v>102.5</v>
+        <v>102.6</v>
       </c>
       <c r="CC3" t="n">
-        <v>101</v>
+        <v>101.17</v>
       </c>
       <c r="CD3" t="n">
-        <v>84.17</v>
+        <v>84.31</v>
       </c>
       <c r="CE3" t="n">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="CF3" t="n">
         <v>0.501</v>
@@ -3139,7 +3139,7 @@
         <v>22</v>
       </c>
       <c r="CR3" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="CS3" t="n">
         <v>25</v>
@@ -3203,7 +3203,7 @@
         <v>0.15</v>
       </c>
       <c r="DL3" t="n">
-        <v>0.279</v>
+        <v>0.276</v>
       </c>
       <c r="DM3" t="n">
         <v>0.549</v>
@@ -3212,7 +3212,7 @@
         <v>0.241</v>
       </c>
       <c r="DO3" t="n">
-        <v>0.171</v>
+        <v>0.173</v>
       </c>
       <c r="DP3" t="n">
         <v>0.293</v>
@@ -3242,7 +3242,7 @@
         <v>14</v>
       </c>
       <c r="DY3" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="DZ3" t="n">
         <v>22</v>
@@ -3518,7 +3518,7 @@
         <v>48</v>
       </c>
       <c r="HI3" t="n">
-        <v>109.7</v>
+        <v>109.5</v>
       </c>
       <c r="HJ3" t="n">
         <v>31.3</v>
@@ -3648,16 +3648,16 @@
         <v>9.699999999999999</v>
       </c>
       <c r="IY3" t="n">
-        <v>33.8</v>
+        <v>34</v>
       </c>
       <c r="IZ3" t="n">
-        <v>43.5</v>
+        <v>43.7</v>
       </c>
       <c r="JA3" t="n">
         <v>22.3</v>
       </c>
       <c r="JB3" t="n">
-        <v>17.3</v>
+        <v>17.5</v>
       </c>
       <c r="JC3" t="n">
         <v>7.7</v>
@@ -3726,7 +3726,7 @@
         <v>16</v>
       </c>
       <c r="JY3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="JZ3" t="n">
         <v>11</v>
@@ -3735,7 +3735,7 @@
         <v>4</v>
       </c>
       <c r="KB3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="KC3" t="n">
         <v>14</v>
@@ -6686,7 +6686,7 @@
         <v>11</v>
       </c>
       <c r="AS7" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AT7" t="n">
         <v>11</v>
@@ -7267,7 +7267,7 @@
         <v>5</v>
       </c>
       <c r="HX7" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="HY7" t="n">
         <v>18</v>
@@ -9386,16 +9386,16 @@
         <v>12.4</v>
       </c>
       <c r="S10" t="n">
-        <v>35.8</v>
+        <v>36</v>
       </c>
       <c r="T10" t="n">
-        <v>48.2</v>
+        <v>48.4</v>
       </c>
       <c r="U10" t="n">
         <v>23.2</v>
       </c>
       <c r="V10" t="n">
-        <v>16.2</v>
+        <v>16.4</v>
       </c>
       <c r="W10" t="n">
         <v>7.6</v>
@@ -9467,13 +9467,13 @@
         <v>14</v>
       </c>
       <c r="AT10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AU10" t="n">
         <v>19</v>
       </c>
       <c r="AV10" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AW10" t="n">
         <v>19</v>
@@ -9528,19 +9528,19 @@
         <v>250</v>
       </c>
       <c r="BM10" t="n">
-        <v>100.8</v>
+        <v>100.6</v>
       </c>
       <c r="BN10" t="n">
-        <v>103.2</v>
+        <v>103</v>
       </c>
       <c r="BO10" t="n">
         <v>107.5</v>
       </c>
       <c r="BP10" t="n">
-        <v>108.9</v>
+        <v>108.7</v>
       </c>
       <c r="BQ10" t="n">
-        <v>-6.7</v>
+        <v>-6.9</v>
       </c>
       <c r="BR10" t="n">
         <v>-5.6</v>
@@ -9549,7 +9549,7 @@
         <v>0.583</v>
       </c>
       <c r="BT10" t="n">
-        <v>1.43</v>
+        <v>1.41</v>
       </c>
       <c r="BU10" t="n">
         <v>16.1</v>
@@ -9558,13 +9558,13 @@
         <v>0.282</v>
       </c>
       <c r="BW10" t="n">
-        <v>0.76</v>
+        <v>0.764</v>
       </c>
       <c r="BX10" t="n">
-        <v>0.503</v>
+        <v>0.505</v>
       </c>
       <c r="BY10" t="n">
-        <v>0.154</v>
+        <v>0.156</v>
       </c>
       <c r="BZ10" t="n">
         <v>0.489</v>
@@ -9573,16 +9573,16 @@
         <v>0.522</v>
       </c>
       <c r="CB10" t="n">
-        <v>103</v>
+        <v>103.1</v>
       </c>
       <c r="CC10" t="n">
-        <v>101.18</v>
+        <v>101.38</v>
       </c>
       <c r="CD10" t="n">
-        <v>84.31999999999999</v>
+        <v>84.48</v>
       </c>
       <c r="CE10" t="n">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="CF10" t="n">
         <v>0.453</v>
@@ -9606,7 +9606,7 @@
         <v>23</v>
       </c>
       <c r="CM10" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="CN10" t="n">
         <v>25</v>
@@ -9615,7 +9615,7 @@
         <v>20</v>
       </c>
       <c r="CP10" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="CQ10" t="n">
         <v>23</v>
@@ -9630,7 +9630,7 @@
         <v>11</v>
       </c>
       <c r="CU10" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="CV10" t="n">
         <v>28</v>
@@ -9682,7 +9682,7 @@
         <v>0.241</v>
       </c>
       <c r="DK10" t="n">
-        <v>0.154</v>
+        <v>0.156</v>
       </c>
       <c r="DL10" t="n">
         <v>0.282</v>
@@ -9694,10 +9694,10 @@
         <v>0.327</v>
       </c>
       <c r="DO10" t="n">
-        <v>0.159</v>
+        <v>0.158</v>
       </c>
       <c r="DP10" t="n">
-        <v>0.24</v>
+        <v>0.236</v>
       </c>
       <c r="DQ10" t="n">
         <v>9</v>
@@ -9721,7 +9721,7 @@
         <v>18</v>
       </c>
       <c r="DX10" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="DY10" t="n">
         <v>8</v>
@@ -10000,13 +10000,13 @@
         <v>50</v>
       </c>
       <c r="HI10" t="n">
-        <v>108.9</v>
+        <v>108.7</v>
       </c>
       <c r="HJ10" t="n">
-        <v>35.8</v>
+        <v>36</v>
       </c>
       <c r="HK10" t="n">
-        <v>0.76</v>
+        <v>0.764</v>
       </c>
       <c r="HL10" t="n">
         <v>7.6</v>
@@ -10042,7 +10042,7 @@
         <v>1</v>
       </c>
       <c r="HW10" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="HX10" t="n">
         <v>14</v>
@@ -11143,7 +11143,7 @@
         <v>14</v>
       </c>
       <c r="KB11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="KC11" t="n">
         <v>16</v>
@@ -14097,13 +14097,13 @@
         <v>2</v>
       </c>
       <c r="AT15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AU15" t="n">
         <v>7</v>
       </c>
       <c r="AV15" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AW15" t="n">
         <v>26</v>
@@ -14251,7 +14251,7 @@
         <v>8</v>
       </c>
       <c r="CR15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="CS15" t="n">
         <v>4</v>
@@ -14354,7 +14354,7 @@
         <v>21</v>
       </c>
       <c r="DY15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="DZ15" t="n">
         <v>7</v>
@@ -16088,7 +16088,7 @@
         <v>26</v>
       </c>
       <c r="CM17" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="CN17" t="n">
         <v>26</v>
@@ -16524,7 +16524,7 @@
         <v>9</v>
       </c>
       <c r="HW17" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="HX17" t="n">
         <v>21</v>
@@ -18727,7 +18727,7 @@
         <v>6</v>
       </c>
       <c r="AT20" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AU20" t="n">
         <v>29</v>
@@ -21502,7 +21502,7 @@
         <v>8</v>
       </c>
       <c r="AS23" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AT23" t="n">
         <v>10</v>
@@ -22083,7 +22083,7 @@
         <v>14</v>
       </c>
       <c r="HX23" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="HY23" t="n">
         <v>11</v>
@@ -22431,7 +22431,7 @@
         <v>1</v>
       </c>
       <c r="AT24" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AU24" t="n">
         <v>24</v>
@@ -25363,7 +25363,7 @@
         <v>15</v>
       </c>
       <c r="CR27" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="CS27" t="n">
         <v>2</v>
@@ -25466,7 +25466,7 @@
         <v>7</v>
       </c>
       <c r="DY27" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="DZ27" t="n">
         <v>24</v>
@@ -28135,7 +28135,7 @@
         <v>28</v>
       </c>
       <c r="CP30" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="CQ30" t="n">
         <v>27</v>
@@ -28919,7 +28919,7 @@
         <v>2</v>
       </c>
       <c r="AV31" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AW31" t="n">
         <v>23</v>
@@ -29076,7 +29076,7 @@
         <v>21</v>
       </c>
       <c r="CU31" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="CV31" t="n">
         <v>7</v>
@@ -29167,7 +29167,7 @@
         <v>9</v>
       </c>
       <c r="DX31" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="DY31" t="n">
         <v>24</v>

</xml_diff>